<commit_message>
some changes in lab_2
</commit_message>
<xml_diff>
--- a/lab_2/docs/pomiary.xlsx
+++ b/lab_2/docs/pomiary.xlsx
@@ -83,8 +83,9 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="11" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -603,6 +604,7 @@
     <col customWidth="1" min="3" max="3" width="26.36328125"/>
     <col customWidth="1" min="4" max="4" width="24.99609375"/>
     <col customWidth="1" min="5" max="5" width="17.0859375"/>
+    <col customWidth="1" min="6" max="6" width="13.140625"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
@@ -654,6 +656,10 @@
       <c r="D4">
         <v>0.265403</v>
       </c>
+      <c r="F4" s="1">
+        <f>B4/1000</f>
+        <v>0.00042966599999999999</v>
+      </c>
     </row>
     <row r="6" ht="14.25">
       <c r="C6" t="s">
@@ -703,14 +709,12 @@
       </c>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11"/>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
       </c>
-      <c r="D11"/>
     </row>
     <row r="12" ht="14.25">
       <c r="A12" t="s">
@@ -753,20 +757,16 @@
       <c r="D14">
         <v>0.019460999999999999</v>
       </c>
-    </row>
-    <row r="15" ht="14.25">
-      <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15"/>
-    </row>
+      <c r="F14" s="1">
+        <f>B14/1000</f>
+        <v>1.6249e-05</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25"/>
     <row r="16" ht="14.25">
-      <c r="A16"/>
-      <c r="B16"/>
       <c r="C16" t="s">
         <v>5</v>
       </c>
-      <c r="D16"/>
     </row>
     <row r="17" ht="14.25">
       <c r="A17" t="s">

</xml_diff>